<commit_message>
Criou o notebook dispersao_ticegov_pib
</commit_message>
<xml_diff>
--- a/eda/ict_in_government/ict_in_government.xlsx
+++ b/eda/ict_in_government/ict_in_government.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lazar\Master-Dissertation\eda\ict_in_government\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{166F16A9-774C-4256-9869-63786424CD4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4E72769-5F5F-4876-8BE5-9445014AEF87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A797439B-AEA8-40E0-9DF5-3355A33859B8}"/>
   </bookViews>
@@ -620,12 +620,6 @@
     <t>Leba0n</t>
   </si>
   <si>
-    <t>0rth Macedonia</t>
-  </si>
-  <si>
-    <t>0rway</t>
-  </si>
-  <si>
     <t>San Mari0</t>
   </si>
   <si>
@@ -633,6 +627,12 @@
   </si>
   <si>
     <t>Indicator_1</t>
+  </si>
+  <si>
+    <t>North Macedonia</t>
+  </si>
+  <si>
+    <t>Norway</t>
   </si>
 </sst>
 </file>
@@ -1028,8 +1028,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03CA1379-AF74-4B20-A165-387FB29030F4}">
   <dimension ref="A1:E387"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="A128" sqref="A128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1050,7 +1050,7 @@
         <v>189</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>190</v>
@@ -3203,7 +3203,7 @@
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A128" s="4" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="B128" s="4">
         <v>2022</v>
@@ -3220,7 +3220,7 @@
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A129" s="4" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="B129" s="4">
         <v>2022</v>
@@ -3577,7 +3577,7 @@
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A150" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B150" s="4">
         <v>2022</v>
@@ -4155,7 +4155,7 @@
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A184" s="4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B184" s="4">
         <v>2022</v>
@@ -6484,7 +6484,7 @@
     </row>
     <row r="321" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A321" s="3" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="B321" s="3">
         <v>2024</v>
@@ -6501,7 +6501,7 @@
     </row>
     <row r="322" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A322" s="3" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="B322" s="3">
         <v>2024</v>
@@ -6858,7 +6858,7 @@
     </row>
     <row r="343" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A343" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B343" s="3">
         <v>2024</v>
@@ -7436,7 +7436,7 @@
     </row>
     <row r="377" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A377" s="3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B377" s="3">
         <v>2024</v>

</xml_diff>